<commit_message>
end 26 new 8
</commit_message>
<xml_diff>
--- a/uloha26/uloha_26.xlsx
+++ b/uloha26/uloha_26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nemec\david\school\praktika\uloha26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205BA5A4-4FB1-4A45-9DF0-CB2C697DE68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C98D47-257A-4A5D-99D4-27EEB98928F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FC616D70-4F2F-4504-8E2C-2C67408ED36D}"/>
   </bookViews>
@@ -36,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
   <si>
     <t>V (ml)</t>
   </si>
@@ -124,6 +146,9 @@
   </si>
   <si>
     <t>číslo měření</t>
+  </si>
+  <si>
+    <t>molární vodivost CH3COOH</t>
   </si>
 </sst>
 </file>
@@ -1432,7 +1457,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>5.2687391516333015</c:v>
+                    <c:v>5.1261935786517796</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1444,7 +1469,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>5.2687391516333015</c:v>
+                    <c:v>5.1261935786517796</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1540,22 +1565,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>321.08256430310877</c:v>
+                  <c:v>311.41093096373464</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>324.01929507417378</c:v>
+                  <c:v>319.18347840448672</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>316.18801301800039</c:v>
+                  <c:v>313.77010468315683</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>320.75626088410155</c:v>
+                  <c:v>319.14432199420582</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>316.92219571076669</c:v>
+                  <c:v>315.71324154334491</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>306.39891044778369</c:v>
+                  <c:v>305.43174711384626</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4728,16 +4753,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5156,8 +5181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6235151B-205D-44F7-BA8D-FE2B8A23E7C1}">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5167,6 +5192,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.77734375" customWidth="1"/>
     <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
@@ -5226,7 +5252,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="I2">
-        <f>H2-$B$26</f>
+        <f t="shared" ref="I2:I7" si="0">H2-$B$26</f>
         <v>31.811999999999998</v>
       </c>
       <c r="J2">
@@ -5245,7 +5271,7 @@
         <v>0.16399999999999998</v>
       </c>
       <c r="N2">
-        <f>SQRT(SUMSQ(M2,$B$29))</f>
+        <f t="shared" ref="N2:N7" si="1">SQRT(SUMSQ(M2,$B$29))</f>
         <v>0.170559091226472</v>
       </c>
       <c r="Q2" t="s">
@@ -5295,33 +5321,33 @@
         <v>2.0430882051282051</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G7" si="0">$D$2*F3*10</f>
+        <f t="shared" ref="G3:G7" si="2">$D$2*F3*10</f>
         <v>0.20430882051282051</v>
       </c>
       <c r="H3">
         <v>66.2</v>
       </c>
       <c r="I3">
-        <f>H3-$B$26</f>
+        <f t="shared" si="0"/>
         <v>65.212000000000003</v>
       </c>
       <c r="J3">
         <v>21.6</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K7" si="1">$C$17/$C$16*F3</f>
+        <f t="shared" ref="K3:K7" si="3">$C$17/$C$16*F3</f>
         <v>3.1797785958779287E-2</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L7" si="2">K3/F3*G3</f>
+        <f t="shared" ref="L3:L7" si="4">K3/F3*G3</f>
         <v>3.1797785958779285E-3</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M7" si="3">0.005*H3</f>
+        <f t="shared" ref="M3:M7" si="5">0.005*H3</f>
         <v>0.33100000000000002</v>
       </c>
       <c r="N3">
-        <f>SQRT(SUMSQ(M3,$B$29))</f>
+        <f t="shared" si="1"/>
         <v>0.33429837510822574</v>
       </c>
       <c r="Q3">
@@ -5342,7 +5368,7 @@
         <v>26.7</v>
       </c>
       <c r="V3">
-        <f>U3-$B$26</f>
+        <f t="shared" ref="V3:V8" si="6">U3-$B$26</f>
         <v>25.712</v>
       </c>
       <c r="W3">
@@ -5361,7 +5387,7 @@
         <v>0.13350000000000001</v>
       </c>
       <c r="AA3">
-        <f>SQRT(SUMSQ(Z3,$B$29))</f>
+        <f t="shared" ref="AA3:AA8" si="7">SQRT(SUMSQ(Z3,$B$29))</f>
         <v>0.14148022335294783</v>
       </c>
     </row>
@@ -5373,7 +5399,7 @@
         <v>1.0462</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C6" si="4">B4</f>
+        <f t="shared" ref="C4:C6" si="8">B4</f>
         <v>1.0462</v>
       </c>
       <c r="E4">
@@ -5384,70 +5410,70 @@
         <v>4.0861764102564102</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.40861764102564102</v>
       </c>
       <c r="H4">
         <v>129.19999999999999</v>
       </c>
       <c r="I4">
-        <f>H4-$B$26</f>
+        <f t="shared" si="0"/>
         <v>128.21199999999999</v>
       </c>
       <c r="J4">
         <v>21.5</v>
       </c>
       <c r="K4">
+        <f t="shared" si="3"/>
+        <v>6.3595571917558574E-2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>6.3595571917558569E-3</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>0.64599999999999991</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="1"/>
-        <v>6.3595571917558574E-2</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>6.3595571917558569E-3</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="3"/>
-        <v>0.64599999999999991</v>
-      </c>
-      <c r="N4">
-        <f>SQRT(SUMSQ(M4,$B$29))</f>
         <v>0.64769622787229497</v>
       </c>
       <c r="R4">
         <v>2</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S8" si="5">F3</f>
+        <f t="shared" ref="S4:S8" si="9">F3</f>
         <v>2.0430882051282051</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T8" si="6">$Q$3*S4*10</f>
+        <f t="shared" ref="T4:T8" si="10">$Q$3*S4*10</f>
         <v>1.0215441025641026</v>
       </c>
       <c r="U4">
         <v>38.799999999999997</v>
       </c>
       <c r="V4">
-        <f>U4-$B$26</f>
+        <f t="shared" si="6"/>
         <v>37.811999999999998</v>
       </c>
       <c r="W4">
         <v>21.6</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X8" si="7">K3</f>
+        <f t="shared" ref="X4:X8" si="11">K3</f>
         <v>3.1797785958779287E-2</v>
       </c>
       <c r="Y4">
-        <f t="shared" ref="Y4:Y8" si="8">X4/S4*T4</f>
+        <f t="shared" ref="Y4:Y8" si="12">X4/S4*T4</f>
         <v>1.5898892979389644E-2</v>
       </c>
       <c r="Z4">
-        <f t="shared" ref="Z4:Z8" si="9">0.005*U4</f>
+        <f t="shared" ref="Z4:Z8" si="13">0.005*U4</f>
         <v>0.19399999999999998</v>
       </c>
       <c r="AA4">
-        <f>SQRT(SUMSQ(Z4,$B$29))</f>
+        <f t="shared" si="7"/>
         <v>0.19957555862379539</v>
       </c>
     </row>
@@ -5459,7 +5485,7 @@
         <v>1.0419</v>
       </c>
       <c r="C5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.0419</v>
       </c>
       <c r="E5">
@@ -5470,70 +5496,70 @@
         <v>6.1292646153846153</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.61292646153846153</v>
       </c>
       <c r="H5">
         <v>196.6</v>
       </c>
       <c r="I5">
-        <f>H5-$B$26</f>
+        <f t="shared" si="0"/>
         <v>195.61199999999999</v>
       </c>
       <c r="J5">
         <v>21.5</v>
       </c>
       <c r="K5">
+        <f t="shared" si="3"/>
+        <v>9.5393357876337861E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>9.5393357876337858E-3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="1"/>
-        <v>9.5393357876337861E-2</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>9.5393357876337858E-3</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="N5">
-        <f>SQRT(SUMSQ(M5,$B$29))</f>
         <v>0.98411554382602862</v>
       </c>
       <c r="R5">
         <v>3</v>
       </c>
       <c r="S5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0861764102564102</v>
       </c>
       <c r="T5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.0430882051282051</v>
       </c>
       <c r="U5">
         <v>55.1</v>
       </c>
       <c r="V5">
-        <f>U5-$B$26</f>
+        <f t="shared" si="6"/>
         <v>54.112000000000002</v>
       </c>
       <c r="W5">
         <v>21.4</v>
       </c>
       <c r="X5">
+        <f t="shared" si="11"/>
+        <v>6.3595571917558574E-2</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="12"/>
+        <v>3.1797785958779287E-2</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="13"/>
+        <v>0.27550000000000002</v>
+      </c>
+      <c r="AA5">
         <f t="shared" si="7"/>
-        <v>6.3595571917558574E-2</v>
-      </c>
-      <c r="Y5">
-        <f t="shared" si="8"/>
-        <v>3.1797785958779287E-2</v>
-      </c>
-      <c r="Z5">
-        <f t="shared" si="9"/>
-        <v>0.27550000000000002</v>
-      </c>
-      <c r="AA5">
-        <f>SQRT(SUMSQ(Z5,$B$29))</f>
         <v>0.27945420662426967</v>
       </c>
     </row>
@@ -5545,7 +5571,7 @@
         <v>1.0362</v>
       </c>
       <c r="C6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.0362</v>
       </c>
       <c r="E6">
@@ -5556,70 +5582,70 @@
         <v>8.1723528205128204</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.81723528205128204</v>
       </c>
       <c r="H6">
         <v>259</v>
       </c>
       <c r="I6">
-        <f>H6-$B$26</f>
+        <f t="shared" si="0"/>
         <v>258.012</v>
       </c>
       <c r="J6">
         <v>21.4</v>
       </c>
       <c r="K6">
+        <f t="shared" si="3"/>
+        <v>0.12719114383511715</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>1.2719114383511714E-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="1"/>
-        <v>0.12719114383511715</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>1.2719114383511714E-2</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>1.2949999999999999</v>
-      </c>
-      <c r="N6">
-        <f>SQRT(SUMSQ(M6,$B$29))</f>
         <v>1.2958469830963839</v>
       </c>
       <c r="R6">
         <v>4</v>
       </c>
       <c r="S6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.1292646153846153</v>
       </c>
       <c r="T6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.0646323076923077</v>
       </c>
       <c r="U6">
         <v>69.5</v>
       </c>
       <c r="V6">
-        <f>U6-$B$26</f>
+        <f t="shared" si="6"/>
         <v>68.512</v>
       </c>
       <c r="W6">
         <v>21.6</v>
       </c>
       <c r="X6">
+        <f t="shared" si="11"/>
+        <v>9.5393357876337861E-2</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="12"/>
+        <v>4.7696678938168931E-2</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="13"/>
+        <v>0.34750000000000003</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="7"/>
-        <v>9.5393357876337861E-2</v>
-      </c>
-      <c r="Y6">
-        <f t="shared" si="8"/>
-        <v>4.7696678938168931E-2</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="9"/>
-        <v>0.34750000000000003</v>
-      </c>
-      <c r="AA6">
-        <f>SQRT(SUMSQ(Z6,$B$29))</f>
         <v>0.350643199848507</v>
       </c>
     </row>
@@ -5642,70 +5668,70 @@
         <v>10.215441025641026</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0215441025641026</v>
       </c>
       <c r="H7">
         <v>313</v>
       </c>
       <c r="I7">
-        <f>H7-$B$26</f>
+        <f t="shared" si="0"/>
         <v>312.012</v>
       </c>
       <c r="J7">
         <v>21.3</v>
       </c>
       <c r="K7">
+        <f t="shared" si="3"/>
+        <v>0.15898892979389642</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>1.589889297938964E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>1.5649999999999999</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="1"/>
-        <v>0.15898892979389642</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>1.589889297938964E-2</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>1.5649999999999999</v>
-      </c>
-      <c r="N7">
-        <f>SQRT(SUMSQ(M7,$B$29))</f>
         <v>1.5657009304461691</v>
       </c>
       <c r="R7">
         <v>5</v>
       </c>
       <c r="S7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8.1723528205128204</v>
       </c>
       <c r="T7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.0861764102564102</v>
       </c>
       <c r="U7">
         <v>80.400000000000006</v>
       </c>
       <c r="V7">
-        <f>U7-$B$26</f>
+        <f t="shared" si="6"/>
         <v>79.412000000000006</v>
       </c>
       <c r="W7">
         <v>21.4</v>
       </c>
       <c r="X7">
+        <f t="shared" si="11"/>
+        <v>0.12719114383511715</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="12"/>
+        <v>6.3595571917558574E-2</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="13"/>
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="AA7">
         <f t="shared" si="7"/>
-        <v>0.12719114383511715</v>
-      </c>
-      <c r="Y7">
-        <f t="shared" si="8"/>
-        <v>6.3595571917558574E-2</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="9"/>
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="AA7">
-        <f>SQRT(SUMSQ(Z7,$B$29))</f>
         <v>0.40472015467480743</v>
       </c>
     </row>
@@ -5724,37 +5750,37 @@
         <v>6</v>
       </c>
       <c r="S8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10.215441025641026</v>
       </c>
       <c r="T8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5.1077205128205128</v>
       </c>
       <c r="U8">
         <v>89.4</v>
       </c>
       <c r="V8">
-        <f>U8-$B$26</f>
+        <f t="shared" si="6"/>
         <v>88.412000000000006</v>
       </c>
       <c r="W8">
         <v>21.5</v>
       </c>
       <c r="X8">
+        <f t="shared" si="11"/>
+        <v>0.15898892979389642</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="12"/>
+        <v>7.9494464896948211E-2</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="13"/>
+        <v>0.44700000000000006</v>
+      </c>
+      <c r="AA8">
         <f t="shared" si="7"/>
-        <v>0.15898892979389642</v>
-      </c>
-      <c r="Y8">
-        <f t="shared" si="8"/>
-        <v>7.9494464896948211E-2</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="9"/>
-        <v>0.44700000000000006</v>
-      </c>
-      <c r="AA8">
-        <f>SQRT(SUMSQ(Z8,$B$29))</f>
         <v>0.44944788752423798</v>
       </c>
     </row>
@@ -5766,7 +5792,7 @@
         <v>2.0470999999999999</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C10" si="10">B9/2</f>
+        <f t="shared" ref="C9:C10" si="14">B9/2</f>
         <v>1.02355</v>
       </c>
     </row>
@@ -5778,7 +5804,7 @@
         <v>2.0432999999999999</v>
       </c>
       <c r="C10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.0216499999999999</v>
       </c>
     </row>
@@ -5851,7 +5877,7 @@
         <v>1.0215441025641026</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>26</v>
       </c>
@@ -5860,12 +5886,18 @@
         <v>1.5898892979389644E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f>SQRT(SUMSQ(C17,0.0001))</f>
+        <v>1.5899207463584003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -5873,7 +5905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5884,7 +5916,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -5894,8 +5926,48 @@
       <c r="C22">
         <v>21.7</v>
       </c>
+      <c r="G22" cm="1">
+        <f t="array" ref="G22:S22">TRANSPOSE(A3:A15)</f>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>4</v>
+      </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+      <c r="R22">
+        <v>5</v>
+      </c>
+      <c r="S22">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -5905,8 +5977,48 @@
       <c r="C23">
         <v>21.4</v>
       </c>
+      <c r="G23" cm="1">
+        <f t="array" ref="G23:S23">TRANSPOSE(B3:B15)</f>
+        <v>1.0467</v>
+      </c>
+      <c r="H23">
+        <v>1.0462</v>
+      </c>
+      <c r="I23">
+        <v>1.0419</v>
+      </c>
+      <c r="J23">
+        <v>1.0362</v>
+      </c>
+      <c r="K23">
+        <v>2.0265</v>
+      </c>
+      <c r="L23">
+        <v>2.0251999999999999</v>
+      </c>
+      <c r="M23">
+        <v>2.0470999999999999</v>
+      </c>
+      <c r="N23">
+        <v>2.0432999999999999</v>
+      </c>
+      <c r="O23">
+        <v>3.0133000000000001</v>
+      </c>
+      <c r="P23">
+        <v>4.0475000000000003</v>
+      </c>
+      <c r="Q23">
+        <v>4.0391000000000004</v>
+      </c>
+      <c r="R23">
+        <v>5.0327999999999999</v>
+      </c>
+      <c r="S23">
+        <v>5.0269000000000004</v>
+      </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -5916,8 +6028,48 @@
       <c r="C24">
         <v>21.8</v>
       </c>
+      <c r="G24" cm="1">
+        <f t="array" ref="G24:S24">TRANSPOSE(C3:C15)</f>
+        <v>1.0467</v>
+      </c>
+      <c r="H24">
+        <v>1.0462</v>
+      </c>
+      <c r="I24">
+        <v>1.0419</v>
+      </c>
+      <c r="J24">
+        <v>1.0362</v>
+      </c>
+      <c r="K24">
+        <v>1.01325</v>
+      </c>
+      <c r="L24">
+        <v>1.0125999999999999</v>
+      </c>
+      <c r="M24">
+        <v>1.02355</v>
+      </c>
+      <c r="N24">
+        <v>1.0216499999999999</v>
+      </c>
+      <c r="O24">
+        <v>1.0044333333333333</v>
+      </c>
+      <c r="P24">
+        <v>1.0118750000000001</v>
+      </c>
+      <c r="Q24">
+        <v>1.0097750000000001</v>
+      </c>
+      <c r="R24">
+        <v>1.0065599999999999</v>
+      </c>
+      <c r="S24">
+        <v>1.0053800000000002</v>
+      </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -5928,7 +6080,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B26">
         <f>AVERAGE(B21:B25)</f>
         <v>0.98799999999999988</v>
@@ -5936,8 +6088,11 @@
       <c r="Q26" t="s">
         <v>10</v>
       </c>
+      <c r="V26" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B27">
         <f>SQRT(SUMSQ(B26-B21,B26-B22,B26-B23,B26-B24,B26-B25)/4)</f>
         <v>4.6583258795408505E-2</v>
@@ -5966,8 +6121,20 @@
       <c r="T27" t="s">
         <v>18</v>
       </c>
+      <c r="V27" t="s">
+        <v>11</v>
+      </c>
+      <c r="W27" t="s">
+        <v>19</v>
+      </c>
+      <c r="X27" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B28">
         <f>0.005*B26</f>
         <v>4.9399999999999991E-3</v>
@@ -5982,7 +6149,7 @@
         <v>19</v>
       </c>
       <c r="Q28">
-        <f t="shared" ref="Q28:Q33" si="11">T3^(1/2)</f>
+        <f t="shared" ref="Q28:Q33" si="15">T3^(1/2)</f>
         <v>0.71468318245363183</v>
       </c>
       <c r="R28">
@@ -5997,8 +6164,24 @@
         <f>AA3</f>
         <v>0.14148022335294783</v>
       </c>
+      <c r="V28">
+        <f>1/Q28</f>
+        <v>1.3992213956495043</v>
+      </c>
+      <c r="W28">
+        <f>V3/T3</f>
+        <v>50.339481057082516</v>
+      </c>
+      <c r="X28">
+        <f>S28/Q28*V28</f>
+        <v>2.1776907299514005E-2</v>
+      </c>
+      <c r="Y28">
+        <f>W28*SQRT(SUMSQ(AA3/V3,Y3/T3))</f>
+        <v>0.83098697495567475</v>
+      </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B29">
         <f>SQRT(SUMSQ(B27,B28))</f>
         <v>4.6844461785786419E-2</v>
@@ -6010,208 +6193,288 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:F34" si="12">G2^(1/2)</f>
+        <f t="shared" ref="F29:F34" si="16">G2^(1/2)</f>
         <v>0.31961603566844116</v>
       </c>
       <c r="G29">
-        <f>H2/G2</f>
-        <v>321.08256430310877</v>
+        <f>I2/G2</f>
+        <v>311.41093096373464</v>
       </c>
       <c r="H29">
         <f>L2/F29</f>
         <v>4.9743727488950574E-3</v>
       </c>
       <c r="I29">
-        <f>G29*SQRT(SUMSQ(N2/H2,L2/G2))</f>
-        <v>5.2687391516333015</v>
+        <f>G29*SQRT(SUMSQ(N2/I2,L2/G2))</f>
+        <v>5.1261935786517796</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1.0107146494258914</v>
       </c>
       <c r="R29">
-        <f t="shared" ref="R29:R33" si="13">V4</f>
+        <f t="shared" ref="R29:R33" si="17">V4</f>
         <v>37.811999999999998</v>
       </c>
       <c r="S29">
-        <f t="shared" ref="S29:S33" si="14">Y4/Q29</f>
+        <f t="shared" ref="S29:S33" si="18">Y4/Q29</f>
         <v>1.573034781718121E-2</v>
       </c>
       <c r="T29">
-        <f t="shared" ref="T29:T33" si="15">AA4</f>
+        <f t="shared" ref="T29:T33" si="19">AA4</f>
         <v>0.19957555862379539</v>
       </c>
+      <c r="V29">
+        <f t="shared" ref="V29:V33" si="20">1/Q29</f>
+        <v>0.98939893724506955</v>
+      </c>
+      <c r="W29">
+        <f t="shared" ref="W29:W33" si="21">V4/T4</f>
+        <v>37.014554638503498</v>
+      </c>
+      <c r="X29">
+        <f t="shared" ref="X29:X33" si="22">S29/Q29*V29</f>
+        <v>1.5398598824757173E-2</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ref="Y29:Y33" si="23">W29*SQRT(SUMSQ(AA4/V4,Y4/T4))</f>
+        <v>0.60830542374601004</v>
+      </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E30">
         <v>2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.45200533239423241</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30:G34" si="16">H3/G3</f>
-        <v>324.01929507417378</v>
+        <f t="shared" ref="G30:G34" si="24">I3/G3</f>
+        <v>319.18347840448672</v>
       </c>
       <c r="H30">
-        <f t="shared" ref="H30:H34" si="17">L3/F30</f>
+        <f t="shared" ref="H30:H34" si="25">L3/F30</f>
         <v>7.0348254057865239E-3</v>
       </c>
       <c r="I30">
-        <f t="shared" ref="I30:I34" si="18">G30*SQRT(SUMSQ(N3/H3,L3/G3))</f>
-        <v>5.3017126010263587</v>
+        <f t="shared" ref="I30:I34" si="26">G30*SQRT(SUMSQ(N3/I3,L3/G3))</f>
+        <v>5.2301755508277514</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1.4293663649072637</v>
       </c>
       <c r="R30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>54.112000000000002</v>
       </c>
       <c r="S30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.2246071223903683E-2</v>
       </c>
       <c r="T30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.27945420662426967</v>
       </c>
+      <c r="V30">
+        <f t="shared" si="20"/>
+        <v>0.69961069782475216</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="21"/>
+        <v>26.485395913978387</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="22"/>
+        <v>1.0888453649757003E-2</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="23"/>
+        <v>0.43430880948803019</v>
+      </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E31">
         <v>3</v>
       </c>
       <c r="F31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.63923207133688231</v>
       </c>
       <c r="G31">
-        <f t="shared" si="16"/>
-        <v>316.18801301800039</v>
+        <f t="shared" si="24"/>
+        <v>313.77010468315683</v>
       </c>
       <c r="H31">
+        <f t="shared" si="25"/>
+        <v>9.9487454977901148E-3</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="26"/>
+        <v>5.1341993552362029</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="15"/>
+        <v>1.7506091247598099</v>
+      </c>
+      <c r="R31">
         <f t="shared" si="17"/>
-        <v>9.9487454977901148E-3</v>
-      </c>
-      <c r="I31">
+        <v>68.512</v>
+      </c>
+      <c r="S31">
         <f t="shared" si="18"/>
-        <v>5.1700054171574612</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="11"/>
-        <v>1.7506091247598099</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="13"/>
-        <v>68.512</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="14"/>
         <v>2.7245761640088042E-2</v>
       </c>
       <c r="T31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.350643199848507</v>
       </c>
+      <c r="V31">
+        <f t="shared" si="20"/>
+        <v>0.57122974275437055</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="21"/>
+        <v>22.355699843022954</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="22"/>
+        <v>8.8903851766166091E-3</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="23"/>
+        <v>0.36626459845977133</v>
+      </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E32">
         <v>4</v>
       </c>
       <c r="F32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.78289620099886903</v>
       </c>
       <c r="G32">
-        <f t="shared" si="16"/>
-        <v>320.75626088410155</v>
+        <f t="shared" si="24"/>
+        <v>319.14432199420582</v>
       </c>
       <c r="H32">
+        <f t="shared" si="25"/>
+        <v>1.2184675025198604E-2</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="26"/>
+        <v>5.220091425748234</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="15"/>
+        <v>2.0214292988517828</v>
+      </c>
+      <c r="R32">
         <f t="shared" si="17"/>
-        <v>1.2184675025198604E-2</v>
-      </c>
-      <c r="I32">
+        <v>79.412000000000006</v>
+      </c>
+      <c r="S32">
         <f t="shared" si="18"/>
-        <v>5.2439684605624386</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="11"/>
-        <v>2.0214292988517828</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="13"/>
-        <v>79.412000000000006</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="14"/>
         <v>3.1460695634362421E-2</v>
       </c>
       <c r="T32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.40472015467480743</v>
       </c>
+      <c r="V32">
+        <f t="shared" si="20"/>
+        <v>0.49469946862253478</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="21"/>
+        <v>19.434305332651277</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="22"/>
+        <v>7.6992994123785867E-3</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="23"/>
+        <v>0.31827152454762297</v>
+      </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.3">
       <c r="E33">
         <v>5</v>
       </c>
       <c r="F33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.90401066478846481</v>
       </c>
       <c r="G33">
-        <f t="shared" si="16"/>
-        <v>316.92219571076669</v>
+        <f t="shared" si="24"/>
+        <v>315.71324154334491</v>
       </c>
       <c r="H33">
+        <f t="shared" si="25"/>
+        <v>1.4069650811573048E-2</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="26"/>
+        <v>5.1631434035078776</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="15"/>
+        <v>2.2600266619711618</v>
+      </c>
+      <c r="R33">
         <f t="shared" si="17"/>
-        <v>1.4069650811573048E-2</v>
-      </c>
-      <c r="I33">
+        <v>88.412000000000006</v>
+      </c>
+      <c r="S33">
         <f t="shared" si="18"/>
-        <v>5.1810530133021802</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="11"/>
-        <v>2.2600266619711618</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="13"/>
-        <v>88.412000000000006</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="14"/>
         <v>3.517412702893262E-2</v>
       </c>
       <c r="T33">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.44944788752423798</v>
       </c>
+      <c r="V33">
+        <f t="shared" si="20"/>
+        <v>0.44247265610920483</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="21"/>
+        <v>17.309482728760035</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="22"/>
+        <v>6.8864627460810826E-3</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="23"/>
+        <v>0.28340434922113417</v>
+      </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.3">
       <c r="E34">
         <v>6</v>
       </c>
       <c r="F34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0107146494258914</v>
       </c>
       <c r="G34">
-        <f t="shared" si="16"/>
-        <v>306.39891044778369</v>
+        <f t="shared" si="24"/>
+        <v>305.43174711384626</v>
       </c>
       <c r="H34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>1.5730347817181207E-2</v>
       </c>
       <c r="I34">
-        <f t="shared" si="18"/>
-        <v>5.0089213956521386</v>
+        <f t="shared" si="26"/>
+        <v>4.9945929860626173</v>
       </c>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>12</v>
       </c>

</xml_diff>